<commit_message>
Track Of Barani.xlsx updated
</commit_message>
<xml_diff>
--- a/Track Of Barani.xlsx
+++ b/Track Of Barani.xlsx
@@ -1285,7 +1285,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="HM1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="HM8" sqref="HM8"/>
+      <selection pane="topRight" activeCell="HM13" sqref="HM13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2593,7 +2593,7 @@
       <c r="HH3" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="HM3" s="2" t="s">
+      <c r="HM3" s="4" t="s">
         <v>170</v>
       </c>
     </row>
@@ -2782,7 +2782,7 @@
       <c r="HH4" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="HM4" s="2" t="s">
+      <c r="HM4" s="4" t="s">
         <v>171</v>
       </c>
     </row>
@@ -2883,7 +2883,7 @@
       <c r="HH5" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="HM5" s="2" t="s">
+      <c r="HM5" s="4" t="s">
         <v>172</v>
       </c>
     </row>

</xml_diff>